<commit_message>
Added language switcher and translation to PL and UA language
</commit_message>
<xml_diff>
--- a/Language.xlsx
+++ b/Language.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>EN</t>
   </si>
@@ -94,6 +94,45 @@
   </si>
   <si>
     <t>Motyw jasny</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>Контакти</t>
+  </si>
+  <si>
+    <t>Фільтрувати контакти</t>
+  </si>
+  <si>
+    <t>Перетворити в xml</t>
+  </si>
+  <si>
+    <t>Ім'я</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>Група</t>
+  </si>
+  <si>
+    <t>Редагувати контакт</t>
+  </si>
+  <si>
+    <t>Видалити контакт</t>
+  </si>
+  <si>
+    <t>Додати контакт</t>
+  </si>
+  <si>
+    <t>Темна тема</t>
+  </si>
+  <si>
+    <t>Мова</t>
+  </si>
+  <si>
+    <t>Світла тема</t>
   </si>
 </sst>
 </file>
@@ -461,149 +500,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="2" max="4" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>